<commit_message>
Add rating for a2
</commit_message>
<xml_diff>
--- a/cleaned_output.xlsx
+++ b/cleaned_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M562"/>
+  <dimension ref="A1:M563"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29099,6 +29099,45 @@
         <v>0</v>
       </c>
     </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>a2</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr"/>
+      <c r="C563" t="inlineStr"/>
+      <c r="D563" t="inlineStr"/>
+      <c r="E563" t="inlineStr">
+        <is>
+          <t>Budget</t>
+        </is>
+      </c>
+      <c r="F563" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G563" t="n">
+        <v>1</v>
+      </c>
+      <c r="H563" t="n">
+        <v>5</v>
+      </c>
+      <c r="I563" t="n">
+        <v>0</v>
+      </c>
+      <c r="J563" t="n">
+        <v>0</v>
+      </c>
+      <c r="K563" t="n">
+        <v>0</v>
+      </c>
+      <c r="L563" t="n">
+        <v>0</v>
+      </c>
+      <c r="M563" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add rating for 44
</commit_message>
<xml_diff>
--- a/cleaned_output.xlsx
+++ b/cleaned_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M563"/>
+  <dimension ref="A1:M564"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29138,6 +29138,45 @@
         <v>0</v>
       </c>
     </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr"/>
+      <c r="C564" t="inlineStr"/>
+      <c r="D564" t="inlineStr"/>
+      <c r="E564" t="inlineStr">
+        <is>
+          <t>Budget</t>
+        </is>
+      </c>
+      <c r="F564" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G564" t="n">
+        <v>1</v>
+      </c>
+      <c r="H564" t="n">
+        <v>0</v>
+      </c>
+      <c r="I564" t="n">
+        <v>0</v>
+      </c>
+      <c r="J564" t="n">
+        <v>0</v>
+      </c>
+      <c r="K564" t="n">
+        <v>0</v>
+      </c>
+      <c r="L564" t="n">
+        <v>0</v>
+      </c>
+      <c r="M564" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add rating for d
</commit_message>
<xml_diff>
--- a/cleaned_output.xlsx
+++ b/cleaned_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M564"/>
+  <dimension ref="A1:M565"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29177,6 +29177,57 @@
         <v>0</v>
       </c>
     </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E565" t="inlineStr">
+        <is>
+          <t>Mid-range</t>
+        </is>
+      </c>
+      <c r="F565" t="n">
+        <v>4</v>
+      </c>
+      <c r="G565" t="n">
+        <v>0</v>
+      </c>
+      <c r="H565" t="n">
+        <v>0</v>
+      </c>
+      <c r="I565" t="n">
+        <v>0</v>
+      </c>
+      <c r="J565" t="n">
+        <v>0</v>
+      </c>
+      <c r="K565" t="n">
+        <v>0</v>
+      </c>
+      <c r="L565" t="n">
+        <v>0</v>
+      </c>
+      <c r="M565" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add rating for test3
</commit_message>
<xml_diff>
--- a/cleaned_output.xlsx
+++ b/cleaned_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M565"/>
+  <dimension ref="A1:M566"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29228,6 +29228,57 @@
         <v>0</v>
       </c>
     </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>test3</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>test3</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>test3</t>
+        </is>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>test3</t>
+        </is>
+      </c>
+      <c r="E566" t="inlineStr">
+        <is>
+          <t>Mid-range</t>
+        </is>
+      </c>
+      <c r="F566" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G566" t="n">
+        <v>1</v>
+      </c>
+      <c r="H566" t="n">
+        <v>5</v>
+      </c>
+      <c r="I566" t="n">
+        <v>0</v>
+      </c>
+      <c r="J566" t="n">
+        <v>0</v>
+      </c>
+      <c r="K566" t="n">
+        <v>0</v>
+      </c>
+      <c r="L566" t="n">
+        <v>0</v>
+      </c>
+      <c r="M566" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add rating for q
</commit_message>
<xml_diff>
--- a/cleaned_output.xlsx
+++ b/cleaned_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M566"/>
+  <dimension ref="A1:M567"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29279,6 +29279,53 @@
         <v>0</v>
       </c>
     </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="D567" t="inlineStr"/>
+      <c r="E567" t="inlineStr">
+        <is>
+          <t>Budget</t>
+        </is>
+      </c>
+      <c r="F567" t="n">
+        <v>1</v>
+      </c>
+      <c r="G567" t="n">
+        <v>0</v>
+      </c>
+      <c r="H567" t="n">
+        <v>0</v>
+      </c>
+      <c r="I567" t="n">
+        <v>0</v>
+      </c>
+      <c r="J567" t="n">
+        <v>0</v>
+      </c>
+      <c r="K567" t="n">
+        <v>0</v>
+      </c>
+      <c r="L567" t="n">
+        <v>0</v>
+      </c>
+      <c r="M567" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add rating for a
</commit_message>
<xml_diff>
--- a/cleaned_output.xlsx
+++ b/cleaned_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M567"/>
+  <dimension ref="A1:M568"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29326,6 +29326,53 @@
         <v>0</v>
       </c>
     </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D568" t="inlineStr"/>
+      <c r="E568" t="inlineStr">
+        <is>
+          <t>Budget</t>
+        </is>
+      </c>
+      <c r="F568" t="n">
+        <v>0</v>
+      </c>
+      <c r="G568" t="n">
+        <v>0</v>
+      </c>
+      <c r="H568" t="n">
+        <v>0</v>
+      </c>
+      <c r="I568" t="n">
+        <v>0</v>
+      </c>
+      <c r="J568" t="n">
+        <v>0</v>
+      </c>
+      <c r="K568" t="n">
+        <v>0</v>
+      </c>
+      <c r="L568" t="n">
+        <v>0</v>
+      </c>
+      <c r="M568" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add rating for s
</commit_message>
<xml_diff>
--- a/cleaned_output.xlsx
+++ b/cleaned_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M568"/>
+  <dimension ref="A1:M569"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29373,6 +29373,57 @@
         <v>0</v>
       </c>
     </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E569" t="inlineStr">
+        <is>
+          <t>Budget (50-150)</t>
+        </is>
+      </c>
+      <c r="F569" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G569" t="n">
+        <v>0</v>
+      </c>
+      <c r="H569" t="n">
+        <v>0</v>
+      </c>
+      <c r="I569" t="n">
+        <v>0</v>
+      </c>
+      <c r="J569" t="n">
+        <v>0</v>
+      </c>
+      <c r="K569" t="n">
+        <v>0</v>
+      </c>
+      <c r="L569" t="n">
+        <v>0</v>
+      </c>
+      <c r="M569" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add rating for Jeddah
</commit_message>
<xml_diff>
--- a/cleaned_output.xlsx
+++ b/cleaned_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M562"/>
+  <dimension ref="A1:M563"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29111,6 +29111,57 @@
         <v>4</v>
       </c>
     </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>Jeddah</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Saudi Arabia</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>A vibrant coastal city on the Red Sea known for its stunning waterfront, rich history, modern lifestyle, diverse cuisine, and its role as the gateway to Makkah.</t>
+        </is>
+      </c>
+      <c r="E563" t="inlineStr">
+        <is>
+          <t>Luxury</t>
+        </is>
+      </c>
+      <c r="F563" t="n">
+        <v>0</v>
+      </c>
+      <c r="G563" t="n">
+        <v>0</v>
+      </c>
+      <c r="H563" t="n">
+        <v>0</v>
+      </c>
+      <c r="I563" t="n">
+        <v>0</v>
+      </c>
+      <c r="J563" t="n">
+        <v>0</v>
+      </c>
+      <c r="K563" t="n">
+        <v>0</v>
+      </c>
+      <c r="L563" t="n">
+        <v>0</v>
+      </c>
+      <c r="M563" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>